<commit_message>
create and edit users
</commit_message>
<xml_diff>
--- a/public/files/Plantilla-Empresa.xlsx
+++ b/public/files/Plantilla-Empresa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alanruizaguirre/Sites/Job/Brainbox/AsientoContables/public/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20DA40EB-9A24-DE44-A851-48165B4AC483}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B9A748E-0448-C44D-842D-86DD25367E89}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1980" yWindow="460" windowWidth="28040" windowHeight="16760" xr2:uid="{5E890B20-ED90-7546-A118-F48036C6C859}"/>
   </bookViews>
@@ -25,12 +25,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>RUC</t>
   </si>
   <si>
     <t>EMPRESA</t>
+  </si>
+  <si>
+    <t>DIRECCION</t>
   </si>
 </sst>
 </file>
@@ -420,22 +423,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03EF110B-BEA5-9E41-BE3D-8F9BC9949CB5}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="66.33203125" customWidth="1"/>
-    <col min="2" max="2" width="45.6640625" customWidth="1"/>
+    <col min="1" max="1" width="55" customWidth="1"/>
+    <col min="2" max="2" width="37" customWidth="1"/>
+    <col min="3" max="3" width="54.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>